<commit_message>
Fix Feb2011 Major and Minor
</commit_message>
<xml_diff>
--- a/Git_Hub_Data_Excel/Feb_2011.xlsx
+++ b/Git_Hub_Data_Excel/Feb_2011.xlsx
@@ -2116,8 +2116,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -2169,7 +2170,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2179,6 +2180,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -2199,11 +2201,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Mar_2011" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="c1Feb" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="c1Feb" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Mar_2011" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2475,8 +2477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB1802"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AE19" sqref="AE19"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AK14" sqref="AK14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2601,20 +2603,20 @@
         <v>19</v>
       </c>
       <c r="AK1">
-        <f>COUNTIF(K$2:K$20, "&gt;0.05")</f>
-        <v>1</v>
+        <f>COUNTIF(K$2:K$31, "&gt;0.05")</f>
+        <v>2</v>
       </c>
       <c r="AL1">
-        <f t="shared" ref="AL1:BB1" si="0">COUNTIF(L$2:L$20, "&gt;0.05")</f>
-        <v>2</v>
+        <f t="shared" ref="AL1:BB1" si="0">COUNTIF(L$2:L$31, "&gt;0.05")</f>
+        <v>3</v>
       </c>
       <c r="AM1">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="AN1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AO1">
         <f t="shared" si="0"/>
@@ -2626,7 +2628,7 @@
       </c>
       <c r="AQ1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR1">
         <f t="shared" si="0"/>
@@ -2638,11 +2640,11 @@
       </c>
       <c r="AT1">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="AU1">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AV1">
         <f t="shared" si="0"/>
@@ -2650,11 +2652,11 @@
       </c>
       <c r="AW1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AX1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AY1">
         <f t="shared" si="0"/>
@@ -2662,7 +2664,7 @@
       </c>
       <c r="AZ1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA1">
         <f t="shared" si="0"/>
@@ -2784,84 +2786,84 @@
         <v>8</v>
       </c>
       <c r="AH2">
-        <f>COUNTIF(K$2:K$20, "&gt;0.05")</f>
-        <v>1</v>
-      </c>
-      <c r="AI2">
-        <f>COUNTIF(K$2:K$20, "&lt;=0.05")-COUNTIF(K$2:K$20,"=0")</f>
-        <v>3</v>
-      </c>
-      <c r="AK2">
-        <f>COUNTIF(K$2:K$20, "&lt;=0.05")-COUNTIF(K$2:K$20,"=0")</f>
-        <v>3</v>
-      </c>
-      <c r="AL2">
-        <f t="shared" ref="AL2:BB2" si="3">COUNTIF(L$2:L$20, "&lt;=0.05")-COUNTIF(L$2:L$20,"=0")</f>
-        <v>0</v>
-      </c>
-      <c r="AM2">
+        <f>COUNTIF(K$2:K$31, "&gt;0.05")</f>
+        <v>2</v>
+      </c>
+      <c r="AI2" s="9">
+        <f>COUNTIF(K$2:K$31, "&lt;=0.05")-COUNTIF(K$2:K$20,"=0")</f>
+        <v>13</v>
+      </c>
+      <c r="AK2" s="9">
+        <f>COUNTIF(K$2:K$31, "&lt;=0.05")-COUNTIF(K$2:K$20,"=0")</f>
+        <v>13</v>
+      </c>
+      <c r="AL2" s="9">
+        <f t="shared" ref="AL2:BB2" si="3">COUNTIF(L$2:L$31, "&lt;=0.05")-COUNTIF(L$2:L$20,"=0")</f>
+        <v>10</v>
+      </c>
+      <c r="AM2" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AN2">
+        <v>2</v>
+      </c>
+      <c r="AN2" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AO2">
+        <v>10</v>
+      </c>
+      <c r="AO2" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AP2">
+        <v>11</v>
+      </c>
+      <c r="AP2" s="9">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="AQ2">
+        <v>13</v>
+      </c>
+      <c r="AQ2" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AR2">
+        <v>10</v>
+      </c>
+      <c r="AR2" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AS2">
+        <v>11</v>
+      </c>
+      <c r="AS2" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AT2">
+        <v>11</v>
+      </c>
+      <c r="AT2" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AU2">
+        <v>4</v>
+      </c>
+      <c r="AU2" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AV2">
+        <v>10</v>
+      </c>
+      <c r="AV2" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AW2">
+        <v>11</v>
+      </c>
+      <c r="AW2" s="9">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AX2">
+        <v>11</v>
+      </c>
+      <c r="AX2" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AY2">
+        <v>9</v>
+      </c>
+      <c r="AY2" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AZ2">
+        <v>11</v>
+      </c>
+      <c r="AZ2" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="BA2">
+        <v>9</v>
+      </c>
+      <c r="BA2" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="BB2">
+        <v>11</v>
+      </c>
+      <c r="BB2" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
@@ -2974,12 +2976,12 @@
         <v>10</v>
       </c>
       <c r="AH3">
-        <f>COUNTIF(L$2:L$20, "&gt;0.05")</f>
-        <v>2</v>
-      </c>
-      <c r="AI3">
-        <f>COUNTIF(L$2:L$20, "&lt;=0.05")-COUNTIF(L$2:L$20,"=0")</f>
-        <v>0</v>
+        <f>COUNTIF(L$2:L$31, "&gt;0.05")</f>
+        <v>3</v>
+      </c>
+      <c r="AI3" s="9">
+        <f>COUNTIF(L$2:L$31, "&lt;=0.05")-COUNTIF(L$2:L$20,"=0")</f>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:54" x14ac:dyDescent="0.25">
@@ -3090,12 +3092,12 @@
         <v>11</v>
       </c>
       <c r="AH4">
-        <f>COUNTIF(M$2:M$20, "&gt;0.05")</f>
-        <v>7</v>
-      </c>
-      <c r="AI4">
-        <f>COUNTIF(M$2:M$20, "&lt;=0.05")-COUNTIF(M$2:M$20,"=0")</f>
-        <v>0</v>
+        <f>COUNTIF(M$2:M$31, "&gt;0.05")</f>
+        <v>16</v>
+      </c>
+      <c r="AI4" s="9">
+        <f>COUNTIF(M$2:M$31, "&lt;=0.05")-COUNTIF(M$2:M$20,"=0")</f>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.25">
@@ -3212,12 +3214,12 @@
         <v>351</v>
       </c>
       <c r="AH5">
-        <f>COUNTIF(N$2:N$20, "&gt;0.05")</f>
-        <v>1</v>
-      </c>
-      <c r="AI5">
-        <f>COUNTIF(N$2:N$20, "&lt;=0.05")-COUNTIF(N$2:N$20,"=0")</f>
-        <v>0</v>
+        <f>COUNTIF(N$2:N$31, "&gt;0.05")</f>
+        <v>2</v>
+      </c>
+      <c r="AI5" s="9">
+        <f>COUNTIF(N$2:N$31, "&lt;=0.05")-COUNTIF(N$2:N$20,"=0")</f>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.25">
@@ -3328,12 +3330,12 @@
         <v>12</v>
       </c>
       <c r="AH6">
-        <f>COUNTIF(O$2:O$20, "&gt;0.05")</f>
-        <v>0</v>
-      </c>
-      <c r="AI6">
-        <f>COUNTIF(O$2:O$20, "&lt;=0.05")-COUNTIF(O$2:O$20,"=0")</f>
-        <v>0</v>
+        <f>COUNTIF(O$2:O$31, "&gt;0.05")</f>
+        <v>0</v>
+      </c>
+      <c r="AI6" s="9">
+        <f>COUNTIF(O$2:O$31, "&lt;=0.05")-COUNTIF(O$2:O$20,"=0")</f>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.25">
@@ -3446,12 +3448,12 @@
         <v>456</v>
       </c>
       <c r="AH7">
-        <f>COUNTIF(P$2:P$20, "&gt;0.05")</f>
-        <v>2</v>
-      </c>
-      <c r="AI7">
-        <f>COUNTIF(P$2:P$20, "&lt;=0.05")-COUNTIF(P$2:P$20,"=0")</f>
-        <v>2</v>
+        <f>COUNTIF(P$2:P$31, "&gt;0.05")</f>
+        <v>2</v>
+      </c>
+      <c r="AI7" s="9">
+        <f>COUNTIF(P$2:P$31, "&lt;=0.05")-COUNTIF(P$2:P$20,"=0")</f>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.25">
@@ -3562,12 +3564,12 @@
         <v>36</v>
       </c>
       <c r="AH8">
-        <f>COUNTIF(Q$2:Q$20, "&gt;0.05")</f>
-        <v>0</v>
-      </c>
-      <c r="AI8">
-        <f>COUNTIF(Q$2:Q$20, "&lt;=0.05")-COUNTIF(Q$2:Q$20,"=0")</f>
-        <v>0</v>
+        <f>COUNTIF(Q$2:Q$31, "&gt;0.05")</f>
+        <v>1</v>
+      </c>
+      <c r="AI8" s="9">
+        <f>COUNTIF(Q$2:Q$31, "&lt;=0.05")-COUNTIF(Q$2:Q$20,"=0")</f>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:54" x14ac:dyDescent="0.25">
@@ -3684,12 +3686,12 @@
         <v>676</v>
       </c>
       <c r="AH9">
-        <f>COUNTIF(R$2:R$20, "&gt;0.05")</f>
-        <v>0</v>
-      </c>
-      <c r="AI9">
-        <f>COUNTIF(R$2:R$20, "&lt;=0.05")-COUNTIF(R$2:R$20,"=0")</f>
-        <v>0</v>
+        <f>COUNTIF(R$2:R$31, "&gt;0.05")</f>
+        <v>0</v>
+      </c>
+      <c r="AI9" s="9">
+        <f>COUNTIF(R$2:R$31, "&lt;=0.05")-COUNTIF(R$2:R$20,"=0")</f>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:54" x14ac:dyDescent="0.25">
@@ -3806,12 +3808,12 @@
         <v>677</v>
       </c>
       <c r="AH10">
-        <f>COUNTIF(S$2:S$20, "&gt;0.05")</f>
-        <v>2</v>
-      </c>
-      <c r="AI10">
-        <f>COUNTIF(S$2:S$20, "&lt;=0.05")-COUNTIF(S$2:S$20,"=0")</f>
-        <v>0</v>
+        <f>COUNTIF(S$2:S$31, "&gt;0.05")</f>
+        <v>2</v>
+      </c>
+      <c r="AI10" s="9">
+        <f>COUNTIF(S$2:S$31, "&lt;=0.05")-COUNTIF(S$2:S$20,"=0")</f>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:54" x14ac:dyDescent="0.25">
@@ -3922,12 +3924,12 @@
         <v>9</v>
       </c>
       <c r="AH11">
-        <f>COUNTIF(T$2:T$20, "&gt;0.05")</f>
-        <v>12</v>
-      </c>
-      <c r="AI11">
-        <f>COUNTIF(T$2:T$20, "&lt;=0.05")-COUNTIF(T$2:T$20,"=0")</f>
-        <v>0</v>
+        <f>COUNTIF(T$2:T$31, "&gt;0.05")</f>
+        <v>19</v>
+      </c>
+      <c r="AI11" s="9">
+        <f>COUNTIF(T$2:T$31, "&lt;=0.05")-COUNTIF(T$2:T$20,"=0")</f>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:54" x14ac:dyDescent="0.25">
@@ -4040,12 +4042,12 @@
         <v>314</v>
       </c>
       <c r="AH12">
-        <f>COUNTIF(U$2:U$20, "&gt;0.05")</f>
-        <v>5</v>
-      </c>
-      <c r="AI12">
-        <f>COUNTIF(U$2:U$20, "&lt;=0.05")-COUNTIF(U$2:U$20,"=0")</f>
-        <v>0</v>
+        <f>COUNTIF(U$2:U$31, "&gt;0.05")</f>
+        <v>6</v>
+      </c>
+      <c r="AI12" s="9">
+        <f>COUNTIF(U$2:U$31, "&lt;=0.05")-COUNTIF(U$2:U$20,"=0")</f>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.25">
@@ -4156,12 +4158,12 @@
         <v>455</v>
       </c>
       <c r="AH13">
-        <f>COUNTIF(V$2:V$20, "&gt;0.05")</f>
-        <v>0</v>
-      </c>
-      <c r="AI13">
-        <f>COUNTIF(V$2:V$20, "&lt;=0.05")-COUNTIF(V$2:V$20,"=0")</f>
-        <v>0</v>
+        <f>COUNTIF(V$2:V$31, "&gt;0.05")</f>
+        <v>0</v>
+      </c>
+      <c r="AI13" s="9">
+        <f>COUNTIF(V$2:V$31, "&lt;=0.05")-COUNTIF(V$2:V$20,"=0")</f>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:54" x14ac:dyDescent="0.25">
@@ -4278,12 +4280,12 @@
         <v>350</v>
       </c>
       <c r="AH14">
-        <f>COUNTIF(W$2:W$20, "&gt;0.05")</f>
-        <v>3</v>
-      </c>
-      <c r="AI14">
-        <f>COUNTIF(W$2:W$20, "&lt;=0.05")-COUNTIF(W$2:W$20,"=0")</f>
-        <v>1</v>
+        <f>COUNTIF(W$2:W$31, "&gt;0.05")</f>
+        <v>4</v>
+      </c>
+      <c r="AI14" s="9">
+        <f>COUNTIF(W$2:W$31, "&lt;=0.05")-COUNTIF(W$2:W$20,"=0")</f>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.25">
@@ -4394,12 +4396,12 @@
         <v>351</v>
       </c>
       <c r="AH15">
-        <f>COUNTIF(X$2:X$20, "&gt;0.05")</f>
-        <v>1</v>
-      </c>
-      <c r="AI15">
-        <f>COUNTIF(X$2:X$20, "&lt;=0.05")-COUNTIF(X$2:X$20,"=0")</f>
-        <v>0</v>
+        <f>COUNTIF(X$2:X$31, "&gt;0.05")</f>
+        <v>3</v>
+      </c>
+      <c r="AI15" s="9">
+        <f>COUNTIF(X$2:X$31, "&lt;=0.05")-COUNTIF(X$2:X$20,"=0")</f>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:54" x14ac:dyDescent="0.25">
@@ -4512,12 +4514,12 @@
         <v>12</v>
       </c>
       <c r="AH16">
-        <f>COUNTIF(Y$2:Y$20, "&gt;0.05")</f>
-        <v>0</v>
-      </c>
-      <c r="AI16">
-        <f>COUNTIF(Y$2:Y$20, "&lt;=0.05")-COUNTIF(Y$2:Y$20,"=0")</f>
-        <v>0</v>
+        <f>COUNTIF(Y$2:Y$31, "&gt;0.05")</f>
+        <v>0</v>
+      </c>
+      <c r="AI16" s="9">
+        <f>COUNTIF(Y$2:Y$31, "&lt;=0.05")-COUNTIF(Y$2:Y$20,"=0")</f>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="2:35" x14ac:dyDescent="0.25">
@@ -4628,12 +4630,12 @@
         <v>456</v>
       </c>
       <c r="AH17">
-        <f>COUNTIF(Z$2:Z$20, "&gt;0.05")</f>
-        <v>0</v>
-      </c>
-      <c r="AI17">
-        <f>COUNTIF(Z$2:Z$20, "&lt;=0.05")-COUNTIF(Z$2:Z$20,"=0")</f>
-        <v>0</v>
+        <f>COUNTIF(Z$2:Z$31, "&gt;0.05")</f>
+        <v>2</v>
+      </c>
+      <c r="AI17" s="9">
+        <f>COUNTIF(Z$2:Z$31, "&lt;=0.05")-COUNTIF(Z$2:Z$20,"=0")</f>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="2:35" x14ac:dyDescent="0.25">
@@ -4750,12 +4752,12 @@
         <v>36</v>
       </c>
       <c r="AH18">
-        <f>COUNTIF(AA$2:AA$20, "&gt;0.05")</f>
-        <v>0</v>
-      </c>
-      <c r="AI18">
-        <f>COUNTIF(AA$2:AA$20, "&lt;=0.05")-COUNTIF(AA$2:AA$20,"=0")</f>
-        <v>0</v>
+        <f>COUNTIF(AA$2:AA$31, "&gt;0.05")</f>
+        <v>0</v>
+      </c>
+      <c r="AI18" s="9">
+        <f>COUNTIF(AA$2:AA$31, "&lt;=0.05")-COUNTIF(AA$2:AA$20,"=0")</f>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="2:35" x14ac:dyDescent="0.25">
@@ -4777,10 +4779,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K19" s="1" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K19" s="1"/>
       <c r="L19" s="1" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
@@ -4866,12 +4865,12 @@
         <v>429</v>
       </c>
       <c r="AH19">
-        <f>COUNTIF(AB$2:AB$20, "&gt;0.05")</f>
-        <v>0</v>
-      </c>
-      <c r="AI19">
-        <f>COUNTIF(AB$2:AB$20, "&lt;=0.05")-COUNTIF(AB$2:AB$20,"=0")</f>
-        <v>0</v>
+        <f>COUNTIF(AB$2:AB$31, "&gt;0.05")</f>
+        <v>0</v>
+      </c>
+      <c r="AI19" s="9">
+        <f>COUNTIF(AB$2:AB$31, "&lt;=0.05")-COUNTIF(AB$2:AB$20,"=0")</f>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="2:35" x14ac:dyDescent="0.25">

</xml_diff>